<commit_message>
Updated Project assest list example.xlsx to contain sound assets
</commit_message>
<xml_diff>
--- a/Project assest list example.xlsx
+++ b/Project assest list example.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22111"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2403\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian.erb\Desktop\flatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="11_8D63C379EB3BF428FEB55CB37173B7F42D73F5DA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A1686512-5EBE-4F49-9538-912AAAFC70B2}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Knight+Player" sheetId="1" r:id="rId1"/>
     <sheet name="Background" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>In progress</t>
   </si>
@@ -37,21 +36,9 @@
     <t xml:space="preserve">Knight / Player </t>
   </si>
   <si>
-    <t xml:space="preserve">Sound hit </t>
-  </si>
-  <si>
-    <t>sound death</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t xml:space="preserve">Script health </t>
   </si>
   <si>
-    <t xml:space="preserve">script scene change </t>
-  </si>
-  <si>
     <t xml:space="preserve">Script </t>
   </si>
   <si>
@@ -67,12 +54,6 @@
     <t>Implemented</t>
   </si>
   <si>
-    <t>Kat</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Category </t>
   </si>
   <si>
@@ -85,25 +66,58 @@
     <t>Asset</t>
   </si>
   <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>legs</t>
-  </si>
-  <si>
-    <t>helmet</t>
-  </si>
-  <si>
     <t>Sword</t>
   </si>
   <si>
     <t>Not Started/Assigned To</t>
   </si>
+  <si>
+    <t xml:space="preserve">Script scene change </t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Fly damage sound</t>
+  </si>
+  <si>
+    <t>Boss fly damage sound</t>
+  </si>
+  <si>
+    <t>Armor clink/Take damage/Menu button</t>
+  </si>
+  <si>
+    <t>In game music</t>
+  </si>
+  <si>
+    <t>Jump whoosh</t>
+  </si>
+  <si>
+    <t>Hitting dummy wooden click</t>
+  </si>
+  <si>
+    <t>Windmill creaking</t>
+  </si>
+  <si>
+    <t>Door open</t>
+  </si>
+  <si>
+    <t>Ambient sounds of start/end screen</t>
+  </si>
+  <si>
+    <t>Death oof</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,11 +474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,25 +495,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -516,89 +530,49 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -650,14 +624,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -666,11 +638,9 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -692,10 +662,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -705,21 +675,62 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>10</v>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B8B1AB-95EA-44FA-A76B-280A7F8E29A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -731,21 +742,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0C5AAC1B3A5834698B991C8B7BE0A43" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d8bfae07456ed53bf096f88a87e9c3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c372ca1-4d00-4da0-9d60-1d24f5b7546b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3317282adf720fe49703ecb68c6f20" ns2:_="">
     <xsd:import namespace="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -891,24 +887,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D8B4A51-A72D-4F05-84AE-D0EEBFFC2F6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -924,4 +918,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>